<commit_message>
Updated data from website. Now includes deaths (as from PHAC website).
</commit_message>
<xml_diff>
--- a/canada_covid.xlsx
+++ b/canada_covid.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="9108"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="9108" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="61">
   <si>
     <t>Date</t>
   </si>
@@ -173,6 +173,42 @@
   </si>
   <si>
     <t>MB_prob</t>
+  </si>
+  <si>
+    <t>BC_deaths</t>
+  </si>
+  <si>
+    <t>AB_deaths</t>
+  </si>
+  <si>
+    <t>SK_deaths</t>
+  </si>
+  <si>
+    <t>MB_deaths</t>
+  </si>
+  <si>
+    <t>ON_deaths</t>
+  </si>
+  <si>
+    <t>QC_deaths</t>
+  </si>
+  <si>
+    <t>NL_deaths</t>
+  </si>
+  <si>
+    <t>NB_deaths</t>
+  </si>
+  <si>
+    <t>NS_deaths</t>
+  </si>
+  <si>
+    <t>PEI_deaths</t>
+  </si>
+  <si>
+    <t>Repat_deaths</t>
+  </si>
+  <si>
+    <t>deaths</t>
   </si>
 </sst>
 </file>
@@ -493,7 +529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -526,11 +562,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y28"/>
+  <dimension ref="A1:AJ29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J1" sqref="J1"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -540,7 +576,7 @@
     <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -557,67 +593,100 @@
         <v>18</v>
       </c>
       <c r="F1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>14</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" t="s">
         <v>47</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>48</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P1" t="s">
         <v>20</v>
       </c>
-      <c r="M1" t="s">
+      <c r="Q1" t="s">
         <v>21</v>
       </c>
-      <c r="N1" t="s">
+      <c r="R1" t="s">
+        <v>53</v>
+      </c>
+      <c r="S1" t="s">
         <v>22</v>
       </c>
-      <c r="O1" t="s">
+      <c r="T1" t="s">
         <v>23</v>
       </c>
-      <c r="P1" t="s">
+      <c r="U1" t="s">
+        <v>54</v>
+      </c>
+      <c r="V1" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="W1" t="s">
         <v>25</v>
       </c>
-      <c r="R1" t="s">
+      <c r="X1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y1" t="s">
         <v>26</v>
       </c>
-      <c r="S1" t="s">
+      <c r="Z1" t="s">
         <v>27</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AA1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB1" t="s">
         <v>28</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AC1" t="s">
         <v>29</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AD1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE1" t="s">
         <v>30</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AF1" t="s">
         <v>31</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AG1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH1" t="s">
         <v>32</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AI1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="AJ1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -630,11 +699,11 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="L2">
+      <c r="P2">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -647,11 +716,11 @@
       <c r="D3">
         <v>4</v>
       </c>
-      <c r="L3">
+      <c r="P3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -664,11 +733,11 @@
       <c r="D4">
         <v>4</v>
       </c>
-      <c r="L4">
+      <c r="P4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -681,11 +750,11 @@
       <c r="D5">
         <v>5</v>
       </c>
-      <c r="L5">
+      <c r="P5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -698,11 +767,11 @@
       <c r="D6">
         <v>5</v>
       </c>
-      <c r="L6">
+      <c r="P6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -715,11 +784,11 @@
       <c r="D7">
         <v>6</v>
       </c>
-      <c r="L7">
+      <c r="P7">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -732,11 +801,11 @@
       <c r="D8">
         <v>6</v>
       </c>
-      <c r="L8">
+      <c r="P8">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -749,11 +818,11 @@
       <c r="D9">
         <v>7</v>
       </c>
-      <c r="L9">
+      <c r="P9">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -766,11 +835,11 @@
       <c r="D10">
         <v>7</v>
       </c>
-      <c r="L10">
+      <c r="P10">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -783,11 +852,11 @@
       <c r="D11">
         <v>7</v>
       </c>
-      <c r="L11">
+      <c r="P11">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -800,11 +869,11 @@
       <c r="D12">
         <v>7</v>
       </c>
-      <c r="L12">
+      <c r="P12">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -817,14 +886,14 @@
       <c r="D13">
         <v>8</v>
       </c>
-      <c r="L13">
+      <c r="P13">
         <v>15</v>
       </c>
-      <c r="N13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="S13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -837,14 +906,14 @@
       <c r="D14">
         <v>12</v>
       </c>
-      <c r="L14">
+      <c r="P14">
         <v>20</v>
       </c>
-      <c r="N14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="S14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -857,14 +926,14 @@
       <c r="D15">
         <v>21</v>
       </c>
-      <c r="L15">
+      <c r="P15">
         <v>22</v>
       </c>
-      <c r="N15">
+      <c r="S15">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -877,14 +946,14 @@
       <c r="D16">
         <v>21</v>
       </c>
-      <c r="L16">
+      <c r="P16">
         <v>28</v>
       </c>
-      <c r="N16">
+      <c r="S16">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -897,14 +966,14 @@
       <c r="D17">
         <v>27</v>
       </c>
-      <c r="L17">
+      <c r="P17">
         <v>28</v>
       </c>
-      <c r="N17">
+      <c r="S17">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -917,17 +986,17 @@
       <c r="D18">
         <v>27</v>
       </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="L18">
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="P18">
         <v>31</v>
       </c>
-      <c r="N18">
+      <c r="S18">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -940,17 +1009,17 @@
       <c r="D19">
         <v>32</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>7</v>
       </c>
-      <c r="L19">
-        <v>34</v>
-      </c>
-      <c r="N19">
+      <c r="P19">
+        <v>34</v>
+      </c>
+      <c r="S19">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -963,20 +1032,20 @@
       <c r="D20">
         <v>39</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>14</v>
       </c>
-      <c r="L20">
+      <c r="P20">
         <v>42</v>
       </c>
-      <c r="N20">
+      <c r="S20">
         <v>7</v>
       </c>
-      <c r="X20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="AH20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -992,50 +1061,50 @@
       <c r="E21">
         <v>0</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>19</v>
       </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
       <c r="H21">
         <v>0</v>
       </c>
-      <c r="I21">
-        <v>1</v>
-      </c>
       <c r="J21">
         <v>0</v>
       </c>
       <c r="K21">
         <v>1</v>
       </c>
-      <c r="L21">
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="P21">
         <v>59</v>
       </c>
-      <c r="M21">
-        <v>0</v>
-      </c>
-      <c r="N21">
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="S21">
         <v>13</v>
       </c>
-      <c r="O21">
-        <v>0</v>
-      </c>
-      <c r="R21">
-        <v>0</v>
-      </c>
-      <c r="S21">
-        <v>1</v>
-      </c>
-      <c r="X21">
-        <v>1</v>
+      <c r="T21">
+        <v>0</v>
       </c>
       <c r="Y21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z21">
+        <v>1</v>
+      </c>
+      <c r="AH21">
+        <v>1</v>
+      </c>
+      <c r="AI21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -1051,50 +1120,50 @@
       <c r="E22">
         <v>0</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>29</v>
       </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
       <c r="H22">
         <v>0</v>
       </c>
-      <c r="I22">
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
         <v>2</v>
       </c>
-      <c r="J22">
-        <v>1</v>
-      </c>
-      <c r="K22">
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22">
         <v>3</v>
       </c>
-      <c r="L22">
+      <c r="P22">
         <v>79</v>
       </c>
-      <c r="M22">
-        <v>0</v>
-      </c>
-      <c r="N22">
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="S22">
         <v>17</v>
       </c>
-      <c r="O22">
-        <v>0</v>
-      </c>
-      <c r="R22">
-        <v>1</v>
-      </c>
-      <c r="S22">
-        <v>1</v>
-      </c>
-      <c r="X22">
+      <c r="T22">
+        <v>0</v>
+      </c>
+      <c r="Y22">
+        <v>1</v>
+      </c>
+      <c r="Z22">
+        <v>1</v>
+      </c>
+      <c r="AH22">
         <v>2</v>
       </c>
-      <c r="Y22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="AI22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -1110,68 +1179,68 @@
       <c r="E23">
         <v>0</v>
       </c>
-      <c r="F23">
-        <v>39</v>
-      </c>
       <c r="G23">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="H23">
-        <v>1</v>
-      </c>
-      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23">
         <v>5</v>
       </c>
-      <c r="J23">
+      <c r="M23">
         <v>4</v>
       </c>
-      <c r="K23">
+      <c r="N23">
         <v>3</v>
       </c>
-      <c r="L23">
+      <c r="P23">
         <v>142</v>
       </c>
-      <c r="M23">
-        <v>0</v>
-      </c>
-      <c r="N23">
-        <v>39</v>
-      </c>
-      <c r="O23">
-        <v>0</v>
-      </c>
-      <c r="P23">
-        <v>0</v>
-      </c>
       <c r="Q23">
-        <v>1</v>
-      </c>
-      <c r="R23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S23">
+        <v>39</v>
+      </c>
+      <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <v>1</v>
+      </c>
+      <c r="Y23">
+        <v>1</v>
+      </c>
+      <c r="Z23">
         <v>5</v>
       </c>
-      <c r="T23">
-        <v>0</v>
-      </c>
-      <c r="U23">
+      <c r="AB23">
+        <v>0</v>
+      </c>
+      <c r="AC23">
         <v>3</v>
       </c>
-      <c r="V23">
-        <v>1</v>
-      </c>
-      <c r="W23">
-        <v>0</v>
-      </c>
-      <c r="X23">
+      <c r="AE23">
+        <v>1</v>
+      </c>
+      <c r="AF23">
+        <v>0</v>
+      </c>
+      <c r="AH23">
         <v>4</v>
       </c>
-      <c r="Y23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="AI23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -1187,68 +1256,68 @@
       <c r="E24">
         <v>0</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>74</v>
       </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
       <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="J24">
         <v>2</v>
       </c>
-      <c r="I24">
+      <c r="K24">
         <v>5</v>
       </c>
-      <c r="J24">
+      <c r="M24">
         <v>7</v>
       </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-      <c r="L24">
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="P24">
         <v>177</v>
       </c>
-      <c r="M24">
-        <v>0</v>
-      </c>
-      <c r="N24">
+      <c r="Q24">
+        <v>0</v>
+      </c>
+      <c r="S24">
         <v>50</v>
       </c>
-      <c r="O24">
-        <v>0</v>
-      </c>
-      <c r="P24">
-        <v>0</v>
-      </c>
-      <c r="Q24">
-        <v>1</v>
-      </c>
-      <c r="R24">
+      <c r="T24">
+        <v>0</v>
+      </c>
+      <c r="V24">
+        <v>0</v>
+      </c>
+      <c r="W24">
+        <v>1</v>
+      </c>
+      <c r="Y24">
         <v>2</v>
       </c>
-      <c r="S24">
+      <c r="Z24">
         <v>5</v>
       </c>
-      <c r="T24">
-        <v>0</v>
-      </c>
-      <c r="U24">
+      <c r="AB24">
+        <v>0</v>
+      </c>
+      <c r="AC24">
         <v>5</v>
       </c>
-      <c r="V24">
-        <v>1</v>
-      </c>
-      <c r="W24">
-        <v>0</v>
-      </c>
-      <c r="X24">
+      <c r="AE24">
+        <v>1</v>
+      </c>
+      <c r="AF24">
+        <v>0</v>
+      </c>
+      <c r="AH24">
         <v>8</v>
       </c>
-      <c r="Y24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="AI24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -1264,68 +1333,68 @@
       <c r="E25">
         <v>0</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>97</v>
       </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
       <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="J25">
         <v>2</v>
       </c>
-      <c r="I25">
+      <c r="K25">
         <v>6</v>
       </c>
-      <c r="J25">
+      <c r="M25">
         <v>8</v>
       </c>
-      <c r="K25">
+      <c r="N25">
         <v>7</v>
       </c>
-      <c r="L25">
+      <c r="P25">
         <v>189</v>
       </c>
-      <c r="M25">
-        <v>0</v>
-      </c>
-      <c r="N25">
+      <c r="Q25">
+        <v>0</v>
+      </c>
+      <c r="S25">
         <v>74</v>
       </c>
-      <c r="O25">
-        <v>0</v>
-      </c>
-      <c r="P25">
-        <v>0</v>
-      </c>
-      <c r="Q25">
-        <v>1</v>
-      </c>
-      <c r="R25">
+      <c r="T25">
+        <v>0</v>
+      </c>
+      <c r="V25">
+        <v>0</v>
+      </c>
+      <c r="W25">
+        <v>1</v>
+      </c>
+      <c r="Y25">
         <v>2</v>
       </c>
-      <c r="S25">
+      <c r="Z25">
         <v>6</v>
       </c>
-      <c r="T25">
-        <v>1</v>
-      </c>
-      <c r="U25">
+      <c r="AB25">
+        <v>1</v>
+      </c>
+      <c r="AC25">
         <v>6</v>
       </c>
-      <c r="V25">
-        <v>1</v>
-      </c>
-      <c r="W25">
-        <v>0</v>
-      </c>
-      <c r="X25">
+      <c r="AE25">
+        <v>1</v>
+      </c>
+      <c r="AF25">
+        <v>0</v>
+      </c>
+      <c r="AH25">
         <v>9</v>
       </c>
-      <c r="Y25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="AI25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -1341,68 +1410,68 @@
       <c r="E26">
         <v>0</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>97</v>
       </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
       <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="J26">
         <v>2</v>
       </c>
-      <c r="I26">
+      <c r="K26">
         <v>14</v>
       </c>
-      <c r="J26">
+      <c r="M26">
         <v>15</v>
       </c>
-      <c r="K26">
-        <v>0</v>
-      </c>
-      <c r="L26">
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="P26">
         <v>212</v>
       </c>
-      <c r="M26">
-        <v>0</v>
-      </c>
-      <c r="N26">
+      <c r="Q26">
+        <v>0</v>
+      </c>
+      <c r="S26">
         <v>94</v>
       </c>
-      <c r="O26">
-        <v>0</v>
-      </c>
-      <c r="P26">
-        <v>0</v>
-      </c>
-      <c r="Q26">
+      <c r="T26">
+        <v>0</v>
+      </c>
+      <c r="V26">
+        <v>0</v>
+      </c>
+      <c r="W26">
         <v>3</v>
       </c>
-      <c r="R26">
+      <c r="Y26">
         <v>2</v>
       </c>
-      <c r="S26">
+      <c r="Z26">
         <v>9</v>
       </c>
-      <c r="T26">
+      <c r="AB26">
         <v>3</v>
       </c>
-      <c r="U26">
+      <c r="AC26">
         <v>9</v>
       </c>
-      <c r="V26">
-        <v>1</v>
-      </c>
-      <c r="W26">
-        <v>0</v>
-      </c>
-      <c r="X26">
+      <c r="AE26">
+        <v>1</v>
+      </c>
+      <c r="AF26">
+        <v>0</v>
+      </c>
+      <c r="AH26">
         <v>9</v>
       </c>
-      <c r="Y26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="AI26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -1418,68 +1487,68 @@
       <c r="E27">
         <v>0</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>119</v>
       </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
       <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="J27">
         <v>2</v>
       </c>
-      <c r="I27">
+      <c r="K27">
         <v>14</v>
       </c>
-      <c r="J27">
+      <c r="M27">
         <v>15</v>
       </c>
-      <c r="K27">
-        <v>0</v>
-      </c>
-      <c r="L27">
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="P27">
         <v>257</v>
       </c>
-      <c r="M27">
-        <v>0</v>
-      </c>
-      <c r="N27">
+      <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="S27">
         <v>94</v>
       </c>
-      <c r="O27">
-        <v>0</v>
-      </c>
-      <c r="P27">
-        <v>1</v>
-      </c>
-      <c r="Q27">
+      <c r="T27">
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <v>1</v>
+      </c>
+      <c r="W27">
         <v>2</v>
       </c>
-      <c r="R27">
+      <c r="Y27">
         <v>2</v>
       </c>
-      <c r="S27">
+      <c r="Z27">
         <v>9</v>
       </c>
-      <c r="T27">
+      <c r="AB27">
         <v>5</v>
       </c>
-      <c r="U27">
+      <c r="AC27">
         <v>9</v>
       </c>
-      <c r="V27">
-        <v>1</v>
-      </c>
-      <c r="W27">
-        <v>0</v>
-      </c>
-      <c r="X27">
+      <c r="AE27">
+        <v>1</v>
+      </c>
+      <c r="AF27">
+        <v>0</v>
+      </c>
+      <c r="AH27">
         <v>9</v>
       </c>
-      <c r="Y27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="AI27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -1495,65 +1564,175 @@
       <c r="E28">
         <v>0</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>146</v>
       </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
       <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="J28">
         <v>8</v>
       </c>
-      <c r="I28">
+      <c r="K28">
         <v>12</v>
       </c>
-      <c r="J28">
+      <c r="M28">
         <v>17</v>
       </c>
-      <c r="K28">
-        <v>0</v>
-      </c>
-      <c r="L28">
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="P28">
         <v>258</v>
       </c>
-      <c r="M28">
-        <v>0</v>
-      </c>
-      <c r="N28">
+      <c r="Q28">
+        <v>0</v>
+      </c>
+      <c r="S28">
         <v>121</v>
       </c>
-      <c r="O28">
-        <v>0</v>
-      </c>
-      <c r="P28">
-        <v>1</v>
-      </c>
-      <c r="Q28">
+      <c r="T28">
+        <v>0</v>
+      </c>
+      <c r="V28">
+        <v>1</v>
+      </c>
+      <c r="W28">
         <v>2</v>
       </c>
-      <c r="R28">
+      <c r="Y28">
         <v>7</v>
       </c>
-      <c r="S28">
+      <c r="Z28">
         <v>4</v>
       </c>
-      <c r="T28">
+      <c r="AB28">
         <v>5</v>
       </c>
-      <c r="U28">
+      <c r="AC28">
         <v>9</v>
       </c>
-      <c r="V28">
+      <c r="AE28">
         <v>2</v>
       </c>
-      <c r="W28">
-        <v>0</v>
-      </c>
-      <c r="X28">
+      <c r="AF28">
+        <v>0</v>
+      </c>
+      <c r="AH28">
         <v>10</v>
       </c>
-      <c r="Y28">
+      <c r="AI28">
         <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="1">
+        <v>43911.375</v>
+      </c>
+      <c r="D29">
+        <v>348</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>9</v>
+      </c>
+      <c r="G29">
+        <v>195</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>8</v>
+      </c>
+      <c r="K29">
+        <v>18</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>17</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <v>311</v>
+      </c>
+      <c r="Q29">
+        <v>0</v>
+      </c>
+      <c r="R29">
+        <v>2</v>
+      </c>
+      <c r="S29">
+        <v>139</v>
+      </c>
+      <c r="T29">
+        <v>0</v>
+      </c>
+      <c r="U29">
+        <v>1</v>
+      </c>
+      <c r="V29">
+        <v>3</v>
+      </c>
+      <c r="W29">
+        <v>1</v>
+      </c>
+      <c r="X29">
+        <v>0</v>
+      </c>
+      <c r="Y29">
+        <v>7</v>
+      </c>
+      <c r="Z29">
+        <v>4</v>
+      </c>
+      <c r="AA29">
+        <v>0</v>
+      </c>
+      <c r="AB29">
+        <v>5</v>
+      </c>
+      <c r="AC29">
+        <v>10</v>
+      </c>
+      <c r="AD29">
+        <v>0</v>
+      </c>
+      <c r="AE29">
+        <v>2</v>
+      </c>
+      <c r="AF29">
+        <v>0</v>
+      </c>
+      <c r="AG29">
+        <v>0</v>
+      </c>
+      <c r="AH29">
+        <v>13</v>
+      </c>
+      <c r="AI29">
+        <v>0</v>
+      </c>
+      <c r="AJ29">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1563,10 +1742,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F215"/>
+  <dimension ref="A1:F248"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A203" workbookViewId="0">
+      <selection activeCell="A217" sqref="A217:C248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5876,6 +6055,666 @@
         <v>3</v>
       </c>
     </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A216" t="s">
+        <v>45</v>
+      </c>
+      <c r="B216" t="s">
+        <v>37</v>
+      </c>
+      <c r="C216" s="1">
+        <v>43911.375</v>
+      </c>
+      <c r="D216" t="s">
+        <v>1</v>
+      </c>
+      <c r="E216" t="s">
+        <v>38</v>
+      </c>
+      <c r="F216">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A217" t="s">
+        <v>45</v>
+      </c>
+      <c r="B217" t="s">
+        <v>37</v>
+      </c>
+      <c r="C217" s="1">
+        <v>43911.375</v>
+      </c>
+      <c r="D217" t="s">
+        <v>1</v>
+      </c>
+      <c r="E217" t="s">
+        <v>39</v>
+      </c>
+      <c r="F217">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A218" t="s">
+        <v>45</v>
+      </c>
+      <c r="B218" t="s">
+        <v>37</v>
+      </c>
+      <c r="C218" s="1">
+        <v>43911.375</v>
+      </c>
+      <c r="D218" t="s">
+        <v>1</v>
+      </c>
+      <c r="E218" t="s">
+        <v>60</v>
+      </c>
+      <c r="F218">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A219" t="s">
+        <v>45</v>
+      </c>
+      <c r="B219" t="s">
+        <v>37</v>
+      </c>
+      <c r="C219" s="1">
+        <v>43911.375</v>
+      </c>
+      <c r="D219" t="s">
+        <v>2</v>
+      </c>
+      <c r="E219" t="s">
+        <v>38</v>
+      </c>
+      <c r="F219">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A220" t="s">
+        <v>45</v>
+      </c>
+      <c r="B220" t="s">
+        <v>37</v>
+      </c>
+      <c r="C220" s="1">
+        <v>43911.375</v>
+      </c>
+      <c r="D220" t="s">
+        <v>2</v>
+      </c>
+      <c r="E220" t="s">
+        <v>39</v>
+      </c>
+      <c r="F220">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A221" t="s">
+        <v>45</v>
+      </c>
+      <c r="B221" t="s">
+        <v>37</v>
+      </c>
+      <c r="C221" s="1">
+        <v>43911.375</v>
+      </c>
+      <c r="D221" t="s">
+        <v>2</v>
+      </c>
+      <c r="E221" t="s">
+        <v>60</v>
+      </c>
+      <c r="F221">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A222" t="s">
+        <v>45</v>
+      </c>
+      <c r="B222" t="s">
+        <v>37</v>
+      </c>
+      <c r="C222" s="1">
+        <v>43911.375</v>
+      </c>
+      <c r="D222" t="s">
+        <v>3</v>
+      </c>
+      <c r="E222" t="s">
+        <v>38</v>
+      </c>
+      <c r="F222">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A223" t="s">
+        <v>45</v>
+      </c>
+      <c r="B223" t="s">
+        <v>37</v>
+      </c>
+      <c r="C223" s="1">
+        <v>43911.375</v>
+      </c>
+      <c r="D223" t="s">
+        <v>3</v>
+      </c>
+      <c r="E223" t="s">
+        <v>39</v>
+      </c>
+      <c r="F223">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A224" t="s">
+        <v>45</v>
+      </c>
+      <c r="B224" t="s">
+        <v>37</v>
+      </c>
+      <c r="C224" s="1">
+        <v>43911.375</v>
+      </c>
+      <c r="D224" t="s">
+        <v>3</v>
+      </c>
+      <c r="E224" t="s">
+        <v>60</v>
+      </c>
+      <c r="F224">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A225" t="s">
+        <v>45</v>
+      </c>
+      <c r="B225" t="s">
+        <v>37</v>
+      </c>
+      <c r="C225" s="1">
+        <v>43911.375</v>
+      </c>
+      <c r="D225" t="s">
+        <v>46</v>
+      </c>
+      <c r="E225" t="s">
+        <v>38</v>
+      </c>
+      <c r="F225">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A226" t="s">
+        <v>45</v>
+      </c>
+      <c r="B226" t="s">
+        <v>37</v>
+      </c>
+      <c r="C226" s="1">
+        <v>43911.375</v>
+      </c>
+      <c r="D226" t="s">
+        <v>46</v>
+      </c>
+      <c r="E226" t="s">
+        <v>39</v>
+      </c>
+      <c r="F226">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A227" t="s">
+        <v>45</v>
+      </c>
+      <c r="B227" t="s">
+        <v>37</v>
+      </c>
+      <c r="C227" s="1">
+        <v>43911.375</v>
+      </c>
+      <c r="D227" t="s">
+        <v>46</v>
+      </c>
+      <c r="E227" t="s">
+        <v>60</v>
+      </c>
+      <c r="F227">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A228" t="s">
+        <v>45</v>
+      </c>
+      <c r="B228" t="s">
+        <v>37</v>
+      </c>
+      <c r="C228" s="1">
+        <v>43911.375</v>
+      </c>
+      <c r="D228" t="s">
+        <v>4</v>
+      </c>
+      <c r="E228" t="s">
+        <v>38</v>
+      </c>
+      <c r="F228">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A229" t="s">
+        <v>45</v>
+      </c>
+      <c r="B229" t="s">
+        <v>37</v>
+      </c>
+      <c r="C229" s="1">
+        <v>43911.375</v>
+      </c>
+      <c r="D229" t="s">
+        <v>4</v>
+      </c>
+      <c r="E229" t="s">
+        <v>39</v>
+      </c>
+      <c r="F229">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A230" t="s">
+        <v>45</v>
+      </c>
+      <c r="B230" t="s">
+        <v>37</v>
+      </c>
+      <c r="C230" s="1">
+        <v>43911.375</v>
+      </c>
+      <c r="D230" t="s">
+        <v>4</v>
+      </c>
+      <c r="E230" t="s">
+        <v>60</v>
+      </c>
+      <c r="F230">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A231" t="s">
+        <v>45</v>
+      </c>
+      <c r="B231" t="s">
+        <v>37</v>
+      </c>
+      <c r="C231" s="1">
+        <v>43911.375</v>
+      </c>
+      <c r="D231" t="s">
+        <v>5</v>
+      </c>
+      <c r="E231" t="s">
+        <v>38</v>
+      </c>
+      <c r="F231">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A232" t="s">
+        <v>45</v>
+      </c>
+      <c r="B232" t="s">
+        <v>37</v>
+      </c>
+      <c r="C232" s="1">
+        <v>43911.375</v>
+      </c>
+      <c r="D232" t="s">
+        <v>5</v>
+      </c>
+      <c r="E232" t="s">
+        <v>39</v>
+      </c>
+      <c r="F232">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A233" t="s">
+        <v>45</v>
+      </c>
+      <c r="B233" t="s">
+        <v>37</v>
+      </c>
+      <c r="C233" s="1">
+        <v>43911.375</v>
+      </c>
+      <c r="D233" t="s">
+        <v>5</v>
+      </c>
+      <c r="E233" t="s">
+        <v>60</v>
+      </c>
+      <c r="F233">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A234" t="s">
+        <v>45</v>
+      </c>
+      <c r="B234" t="s">
+        <v>37</v>
+      </c>
+      <c r="C234" s="1">
+        <v>43911.375</v>
+      </c>
+      <c r="D234" t="s">
+        <v>6</v>
+      </c>
+      <c r="E234" t="s">
+        <v>38</v>
+      </c>
+      <c r="F234">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A235" t="s">
+        <v>45</v>
+      </c>
+      <c r="B235" t="s">
+        <v>37</v>
+      </c>
+      <c r="C235" s="1">
+        <v>43911.375</v>
+      </c>
+      <c r="D235" t="s">
+        <v>6</v>
+      </c>
+      <c r="E235" t="s">
+        <v>39</v>
+      </c>
+      <c r="F235">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A236" t="s">
+        <v>45</v>
+      </c>
+      <c r="B236" t="s">
+        <v>37</v>
+      </c>
+      <c r="C236" s="1">
+        <v>43911.375</v>
+      </c>
+      <c r="D236" t="s">
+        <v>6</v>
+      </c>
+      <c r="E236" t="s">
+        <v>60</v>
+      </c>
+      <c r="F236">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A237" t="s">
+        <v>45</v>
+      </c>
+      <c r="B237" t="s">
+        <v>37</v>
+      </c>
+      <c r="C237" s="1">
+        <v>43911.375</v>
+      </c>
+      <c r="D237" t="s">
+        <v>7</v>
+      </c>
+      <c r="E237" t="s">
+        <v>38</v>
+      </c>
+      <c r="F237">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A238" t="s">
+        <v>45</v>
+      </c>
+      <c r="B238" t="s">
+        <v>37</v>
+      </c>
+      <c r="C238" s="1">
+        <v>43911.375</v>
+      </c>
+      <c r="D238" t="s">
+        <v>7</v>
+      </c>
+      <c r="E238" t="s">
+        <v>39</v>
+      </c>
+      <c r="F238">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A239" t="s">
+        <v>45</v>
+      </c>
+      <c r="B239" t="s">
+        <v>37</v>
+      </c>
+      <c r="C239" s="1">
+        <v>43911.375</v>
+      </c>
+      <c r="D239" t="s">
+        <v>7</v>
+      </c>
+      <c r="E239" t="s">
+        <v>60</v>
+      </c>
+      <c r="F239">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A240" t="s">
+        <v>45</v>
+      </c>
+      <c r="B240" t="s">
+        <v>37</v>
+      </c>
+      <c r="C240" s="1">
+        <v>43911.375</v>
+      </c>
+      <c r="D240" t="s">
+        <v>8</v>
+      </c>
+      <c r="E240" t="s">
+        <v>38</v>
+      </c>
+      <c r="F240">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A241" t="s">
+        <v>45</v>
+      </c>
+      <c r="B241" t="s">
+        <v>37</v>
+      </c>
+      <c r="C241" s="1">
+        <v>43911.375</v>
+      </c>
+      <c r="D241" t="s">
+        <v>8</v>
+      </c>
+      <c r="E241" t="s">
+        <v>39</v>
+      </c>
+      <c r="F241">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A242" t="s">
+        <v>45</v>
+      </c>
+      <c r="B242" t="s">
+        <v>37</v>
+      </c>
+      <c r="C242" s="1">
+        <v>43911.375</v>
+      </c>
+      <c r="D242" t="s">
+        <v>8</v>
+      </c>
+      <c r="E242" t="s">
+        <v>60</v>
+      </c>
+      <c r="F242">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A243" t="s">
+        <v>45</v>
+      </c>
+      <c r="B243" t="s">
+        <v>37</v>
+      </c>
+      <c r="C243" s="1">
+        <v>43911.375</v>
+      </c>
+      <c r="D243" t="s">
+        <v>9</v>
+      </c>
+      <c r="E243" t="s">
+        <v>38</v>
+      </c>
+      <c r="F243">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A244" t="s">
+        <v>45</v>
+      </c>
+      <c r="B244" t="s">
+        <v>37</v>
+      </c>
+      <c r="C244" s="1">
+        <v>43911.375</v>
+      </c>
+      <c r="D244" t="s">
+        <v>9</v>
+      </c>
+      <c r="E244" t="s">
+        <v>39</v>
+      </c>
+      <c r="F244">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A245" t="s">
+        <v>45</v>
+      </c>
+      <c r="B245" t="s">
+        <v>37</v>
+      </c>
+      <c r="C245" s="1">
+        <v>43911.375</v>
+      </c>
+      <c r="D245" t="s">
+        <v>9</v>
+      </c>
+      <c r="E245" t="s">
+        <v>60</v>
+      </c>
+      <c r="F245">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A246" t="s">
+        <v>45</v>
+      </c>
+      <c r="B246" t="s">
+        <v>37</v>
+      </c>
+      <c r="C246" s="1">
+        <v>43911.375</v>
+      </c>
+      <c r="D246" t="s">
+        <v>40</v>
+      </c>
+      <c r="E246" t="s">
+        <v>38</v>
+      </c>
+      <c r="F246">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A247" t="s">
+        <v>45</v>
+      </c>
+      <c r="B247" t="s">
+        <v>37</v>
+      </c>
+      <c r="C247" s="1">
+        <v>43911.375</v>
+      </c>
+      <c r="D247" t="s">
+        <v>40</v>
+      </c>
+      <c r="E247" t="s">
+        <v>39</v>
+      </c>
+      <c r="F247">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A248" t="s">
+        <v>45</v>
+      </c>
+      <c r="B248" t="s">
+        <v>37</v>
+      </c>
+      <c r="C248" s="1">
+        <v>43911.375</v>
+      </c>
+      <c r="D248" t="s">
+        <v>40</v>
+      </c>
+      <c r="E248" t="s">
+        <v>60</v>
+      </c>
+      <c r="F248">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated as of March 23 18:00.
</commit_message>
<xml_diff>
--- a/canada_covid.xlsx
+++ b/canada_covid.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1412" uniqueCount="69">
   <si>
     <t>Date</t>
   </si>
@@ -586,11 +586,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AP30"/>
+  <dimension ref="A1:AP31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1905,6 +1905,134 @@
         <v>0</v>
       </c>
     </row>
+    <row r="31" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D31">
+        <v>472</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>13</v>
+      </c>
+      <c r="G31">
+        <v>301</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <v>65</v>
+      </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <v>11</v>
+      </c>
+      <c r="N31">
+        <v>9</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <v>503</v>
+      </c>
+      <c r="Q31">
+        <v>0</v>
+      </c>
+      <c r="R31">
+        <v>6</v>
+      </c>
+      <c r="S31">
+        <v>221</v>
+      </c>
+      <c r="T31">
+        <v>407</v>
+      </c>
+      <c r="U31">
+        <v>4</v>
+      </c>
+      <c r="V31">
+        <v>4</v>
+      </c>
+      <c r="W31">
+        <v>20</v>
+      </c>
+      <c r="X31">
+        <v>0</v>
+      </c>
+      <c r="Y31">
+        <v>9</v>
+      </c>
+      <c r="Z31">
+        <v>8</v>
+      </c>
+      <c r="AA31">
+        <v>0</v>
+      </c>
+      <c r="AB31">
+        <v>41</v>
+      </c>
+      <c r="AC31">
+        <v>0</v>
+      </c>
+      <c r="AD31">
+        <v>0</v>
+      </c>
+      <c r="AE31">
+        <v>3</v>
+      </c>
+      <c r="AF31">
+        <v>0</v>
+      </c>
+      <c r="AG31">
+        <v>0</v>
+      </c>
+      <c r="AH31">
+        <v>13</v>
+      </c>
+      <c r="AI31">
+        <v>0</v>
+      </c>
+      <c r="AJ31">
+        <v>0</v>
+      </c>
+      <c r="AK31">
+        <v>2</v>
+      </c>
+      <c r="AL31">
+        <v>0</v>
+      </c>
+      <c r="AM31">
+        <v>0</v>
+      </c>
+      <c r="AN31">
+        <v>1</v>
+      </c>
+      <c r="AO31">
+        <v>0</v>
+      </c>
+      <c r="AP31">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1912,10 +2040,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F287"/>
+  <dimension ref="A1:F326"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C249" sqref="C249:C287"/>
+    <sheetView tabSelected="1" topLeftCell="A274" workbookViewId="0">
+      <selection activeCell="C288" sqref="C288:C326"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7665,6 +7793,786 @@
         <v>0</v>
       </c>
     </row>
+    <row r="288" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A288" t="s">
+        <v>45</v>
+      </c>
+      <c r="B288" t="s">
+        <v>37</v>
+      </c>
+      <c r="C288" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D288" t="s">
+        <v>1</v>
+      </c>
+      <c r="E288" t="s">
+        <v>38</v>
+      </c>
+      <c r="F288">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A289" t="s">
+        <v>45</v>
+      </c>
+      <c r="B289" t="s">
+        <v>37</v>
+      </c>
+      <c r="C289" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D289" t="s">
+        <v>1</v>
+      </c>
+      <c r="E289" t="s">
+        <v>39</v>
+      </c>
+      <c r="F289">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A290" t="s">
+        <v>45</v>
+      </c>
+      <c r="B290" t="s">
+        <v>37</v>
+      </c>
+      <c r="C290" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D290" t="s">
+        <v>1</v>
+      </c>
+      <c r="E290" t="s">
+        <v>60</v>
+      </c>
+      <c r="F290">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A291" t="s">
+        <v>45</v>
+      </c>
+      <c r="B291" t="s">
+        <v>37</v>
+      </c>
+      <c r="C291" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D291" t="s">
+        <v>2</v>
+      </c>
+      <c r="E291" t="s">
+        <v>38</v>
+      </c>
+      <c r="F291">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A292" t="s">
+        <v>45</v>
+      </c>
+      <c r="B292" t="s">
+        <v>37</v>
+      </c>
+      <c r="C292" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D292" t="s">
+        <v>2</v>
+      </c>
+      <c r="E292" t="s">
+        <v>39</v>
+      </c>
+      <c r="F292">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A293" t="s">
+        <v>45</v>
+      </c>
+      <c r="B293" t="s">
+        <v>37</v>
+      </c>
+      <c r="C293" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D293" t="s">
+        <v>2</v>
+      </c>
+      <c r="E293" t="s">
+        <v>60</v>
+      </c>
+      <c r="F293">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="294" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A294" t="s">
+        <v>45</v>
+      </c>
+      <c r="B294" t="s">
+        <v>37</v>
+      </c>
+      <c r="C294" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D294" t="s">
+        <v>3</v>
+      </c>
+      <c r="E294" t="s">
+        <v>38</v>
+      </c>
+      <c r="F294">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A295" t="s">
+        <v>45</v>
+      </c>
+      <c r="B295" t="s">
+        <v>37</v>
+      </c>
+      <c r="C295" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D295" t="s">
+        <v>3</v>
+      </c>
+      <c r="E295" t="s">
+        <v>39</v>
+      </c>
+      <c r="F295">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="296" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A296" t="s">
+        <v>45</v>
+      </c>
+      <c r="B296" t="s">
+        <v>37</v>
+      </c>
+      <c r="C296" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D296" t="s">
+        <v>3</v>
+      </c>
+      <c r="E296" t="s">
+        <v>60</v>
+      </c>
+      <c r="F296">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="297" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A297" t="s">
+        <v>45</v>
+      </c>
+      <c r="B297" t="s">
+        <v>37</v>
+      </c>
+      <c r="C297" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D297" t="s">
+        <v>46</v>
+      </c>
+      <c r="E297" t="s">
+        <v>38</v>
+      </c>
+      <c r="F297">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A298" t="s">
+        <v>45</v>
+      </c>
+      <c r="B298" t="s">
+        <v>37</v>
+      </c>
+      <c r="C298" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D298" t="s">
+        <v>46</v>
+      </c>
+      <c r="E298" t="s">
+        <v>39</v>
+      </c>
+      <c r="F298">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A299" t="s">
+        <v>45</v>
+      </c>
+      <c r="B299" t="s">
+        <v>37</v>
+      </c>
+      <c r="C299" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D299" t="s">
+        <v>46</v>
+      </c>
+      <c r="E299" t="s">
+        <v>60</v>
+      </c>
+      <c r="F299">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A300" t="s">
+        <v>45</v>
+      </c>
+      <c r="B300" t="s">
+        <v>37</v>
+      </c>
+      <c r="C300" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D300" t="s">
+        <v>4</v>
+      </c>
+      <c r="E300" t="s">
+        <v>38</v>
+      </c>
+      <c r="F300">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="301" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A301" t="s">
+        <v>45</v>
+      </c>
+      <c r="B301" t="s">
+        <v>37</v>
+      </c>
+      <c r="C301" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D301" t="s">
+        <v>4</v>
+      </c>
+      <c r="E301" t="s">
+        <v>39</v>
+      </c>
+      <c r="F301">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="302" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A302" t="s">
+        <v>45</v>
+      </c>
+      <c r="B302" t="s">
+        <v>37</v>
+      </c>
+      <c r="C302" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D302" t="s">
+        <v>4</v>
+      </c>
+      <c r="E302" t="s">
+        <v>60</v>
+      </c>
+      <c r="F302">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A303" t="s">
+        <v>45</v>
+      </c>
+      <c r="B303" t="s">
+        <v>37</v>
+      </c>
+      <c r="C303" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D303" t="s">
+        <v>5</v>
+      </c>
+      <c r="E303" t="s">
+        <v>38</v>
+      </c>
+      <c r="F303">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="304" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A304" t="s">
+        <v>45</v>
+      </c>
+      <c r="B304" t="s">
+        <v>37</v>
+      </c>
+      <c r="C304" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D304" t="s">
+        <v>5</v>
+      </c>
+      <c r="E304" t="s">
+        <v>39</v>
+      </c>
+      <c r="F304">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="305" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A305" t="s">
+        <v>45</v>
+      </c>
+      <c r="B305" t="s">
+        <v>37</v>
+      </c>
+      <c r="C305" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D305" t="s">
+        <v>5</v>
+      </c>
+      <c r="E305" t="s">
+        <v>60</v>
+      </c>
+      <c r="F305">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="306" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A306" t="s">
+        <v>45</v>
+      </c>
+      <c r="B306" t="s">
+        <v>37</v>
+      </c>
+      <c r="C306" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D306" t="s">
+        <v>6</v>
+      </c>
+      <c r="E306" t="s">
+        <v>38</v>
+      </c>
+      <c r="F306">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="307" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A307" t="s">
+        <v>45</v>
+      </c>
+      <c r="B307" t="s">
+        <v>37</v>
+      </c>
+      <c r="C307" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D307" t="s">
+        <v>6</v>
+      </c>
+      <c r="E307" t="s">
+        <v>39</v>
+      </c>
+      <c r="F307">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="308" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A308" t="s">
+        <v>45</v>
+      </c>
+      <c r="B308" t="s">
+        <v>37</v>
+      </c>
+      <c r="C308" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D308" t="s">
+        <v>6</v>
+      </c>
+      <c r="E308" t="s">
+        <v>60</v>
+      </c>
+      <c r="F308">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="309" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A309" t="s">
+        <v>45</v>
+      </c>
+      <c r="B309" t="s">
+        <v>37</v>
+      </c>
+      <c r="C309" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D309" t="s">
+        <v>7</v>
+      </c>
+      <c r="E309" t="s">
+        <v>38</v>
+      </c>
+      <c r="F309">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="310" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A310" t="s">
+        <v>45</v>
+      </c>
+      <c r="B310" t="s">
+        <v>37</v>
+      </c>
+      <c r="C310" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D310" t="s">
+        <v>7</v>
+      </c>
+      <c r="E310" t="s">
+        <v>39</v>
+      </c>
+      <c r="F310">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="311" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A311" t="s">
+        <v>45</v>
+      </c>
+      <c r="B311" t="s">
+        <v>37</v>
+      </c>
+      <c r="C311" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D311" t="s">
+        <v>7</v>
+      </c>
+      <c r="E311" t="s">
+        <v>60</v>
+      </c>
+      <c r="F311">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="312" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A312" t="s">
+        <v>45</v>
+      </c>
+      <c r="B312" t="s">
+        <v>37</v>
+      </c>
+      <c r="C312" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D312" t="s">
+        <v>8</v>
+      </c>
+      <c r="E312" t="s">
+        <v>38</v>
+      </c>
+      <c r="F312">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="313" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A313" t="s">
+        <v>45</v>
+      </c>
+      <c r="B313" t="s">
+        <v>37</v>
+      </c>
+      <c r="C313" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D313" t="s">
+        <v>8</v>
+      </c>
+      <c r="E313" t="s">
+        <v>39</v>
+      </c>
+      <c r="F313">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="314" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A314" t="s">
+        <v>45</v>
+      </c>
+      <c r="B314" t="s">
+        <v>37</v>
+      </c>
+      <c r="C314" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D314" t="s">
+        <v>8</v>
+      </c>
+      <c r="E314" t="s">
+        <v>60</v>
+      </c>
+      <c r="F314">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="315" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A315" t="s">
+        <v>45</v>
+      </c>
+      <c r="B315" t="s">
+        <v>37</v>
+      </c>
+      <c r="C315" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D315" t="s">
+        <v>9</v>
+      </c>
+      <c r="E315" t="s">
+        <v>38</v>
+      </c>
+      <c r="F315">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="316" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A316" t="s">
+        <v>45</v>
+      </c>
+      <c r="B316" t="s">
+        <v>37</v>
+      </c>
+      <c r="C316" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D316" t="s">
+        <v>9</v>
+      </c>
+      <c r="E316" t="s">
+        <v>39</v>
+      </c>
+      <c r="F316">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="317" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A317" t="s">
+        <v>45</v>
+      </c>
+      <c r="B317" t="s">
+        <v>37</v>
+      </c>
+      <c r="C317" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D317" t="s">
+        <v>9</v>
+      </c>
+      <c r="E317" t="s">
+        <v>60</v>
+      </c>
+      <c r="F317">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="318" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A318" t="s">
+        <v>45</v>
+      </c>
+      <c r="B318" t="s">
+        <v>37</v>
+      </c>
+      <c r="C318" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D318" t="s">
+        <v>40</v>
+      </c>
+      <c r="E318" t="s">
+        <v>38</v>
+      </c>
+      <c r="F318">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="319" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A319" t="s">
+        <v>45</v>
+      </c>
+      <c r="B319" t="s">
+        <v>37</v>
+      </c>
+      <c r="C319" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D319" t="s">
+        <v>40</v>
+      </c>
+      <c r="E319" t="s">
+        <v>39</v>
+      </c>
+      <c r="F319">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="320" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A320" t="s">
+        <v>45</v>
+      </c>
+      <c r="B320" t="s">
+        <v>37</v>
+      </c>
+      <c r="C320" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D320" t="s">
+        <v>40</v>
+      </c>
+      <c r="E320" t="s">
+        <v>60</v>
+      </c>
+      <c r="F320">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="321" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A321" t="s">
+        <v>45</v>
+      </c>
+      <c r="B321" t="s">
+        <v>37</v>
+      </c>
+      <c r="C321" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D321" t="s">
+        <v>67</v>
+      </c>
+      <c r="E321" t="s">
+        <v>38</v>
+      </c>
+      <c r="F321">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="322" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A322" t="s">
+        <v>45</v>
+      </c>
+      <c r="B322" t="s">
+        <v>37</v>
+      </c>
+      <c r="C322" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D322" t="s">
+        <v>67</v>
+      </c>
+      <c r="E322" t="s">
+        <v>39</v>
+      </c>
+      <c r="F322">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="323" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A323" t="s">
+        <v>45</v>
+      </c>
+      <c r="B323" t="s">
+        <v>37</v>
+      </c>
+      <c r="C323" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D323" t="s">
+        <v>67</v>
+      </c>
+      <c r="E323" t="s">
+        <v>60</v>
+      </c>
+      <c r="F323">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="324" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A324" t="s">
+        <v>45</v>
+      </c>
+      <c r="B324" t="s">
+        <v>37</v>
+      </c>
+      <c r="C324" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D324" t="s">
+        <v>68</v>
+      </c>
+      <c r="E324" t="s">
+        <v>38</v>
+      </c>
+      <c r="F324">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="325" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A325" t="s">
+        <v>45</v>
+      </c>
+      <c r="B325" t="s">
+        <v>37</v>
+      </c>
+      <c r="C325" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D325" t="s">
+        <v>68</v>
+      </c>
+      <c r="E325" t="s">
+        <v>39</v>
+      </c>
+      <c r="F325">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="326" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A326" t="s">
+        <v>45</v>
+      </c>
+      <c r="B326" t="s">
+        <v>37</v>
+      </c>
+      <c r="C326" s="1">
+        <v>43913.75</v>
+      </c>
+      <c r="D326" t="s">
+        <v>68</v>
+      </c>
+      <c r="E326" t="s">
+        <v>60</v>
+      </c>
+      <c r="F326">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated data as of March 24 18:00.
</commit_message>
<xml_diff>
--- a/canada_covid.xlsx
+++ b/canada_covid.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1412" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1570" uniqueCount="69">
   <si>
     <t>Date</t>
   </si>
@@ -586,11 +586,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AP31"/>
+  <dimension ref="A1:AP32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2033,6 +2033,134 @@
         <v>0</v>
       </c>
     </row>
+    <row r="32" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D32">
+        <v>617</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>13</v>
+      </c>
+      <c r="G32">
+        <v>358</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>2</v>
+      </c>
+      <c r="J32">
+        <v>72</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <v>11</v>
+      </c>
+      <c r="N32">
+        <v>10</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <v>588</v>
+      </c>
+      <c r="Q32">
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <v>8</v>
+      </c>
+      <c r="S32">
+        <v>221</v>
+      </c>
+      <c r="T32">
+        <v>792</v>
+      </c>
+      <c r="U32">
+        <v>4</v>
+      </c>
+      <c r="V32">
+        <v>4</v>
+      </c>
+      <c r="W32">
+        <v>31</v>
+      </c>
+      <c r="X32">
+        <v>0</v>
+      </c>
+      <c r="Y32">
+        <v>18</v>
+      </c>
+      <c r="Z32">
+        <v>0</v>
+      </c>
+      <c r="AA32">
+        <v>0</v>
+      </c>
+      <c r="AB32">
+        <v>51</v>
+      </c>
+      <c r="AC32">
+        <v>0</v>
+      </c>
+      <c r="AD32">
+        <v>0</v>
+      </c>
+      <c r="AE32">
+        <v>3</v>
+      </c>
+      <c r="AF32">
+        <v>0</v>
+      </c>
+      <c r="AG32">
+        <v>0</v>
+      </c>
+      <c r="AH32">
+        <v>13</v>
+      </c>
+      <c r="AI32">
+        <v>0</v>
+      </c>
+      <c r="AJ32">
+        <v>0</v>
+      </c>
+      <c r="AK32">
+        <v>2</v>
+      </c>
+      <c r="AL32">
+        <v>0</v>
+      </c>
+      <c r="AM32">
+        <v>0</v>
+      </c>
+      <c r="AN32">
+        <v>1</v>
+      </c>
+      <c r="AO32">
+        <v>0</v>
+      </c>
+      <c r="AP32">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2040,10 +2168,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F326"/>
+  <dimension ref="A1:F365"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A274" workbookViewId="0">
-      <selection activeCell="C288" sqref="C288:C326"/>
+    <sheetView tabSelected="1" topLeftCell="A313" workbookViewId="0">
+      <selection activeCell="A327" sqref="A327:C365"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8573,6 +8701,786 @@
         <v>0</v>
       </c>
     </row>
+    <row r="327" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A327" t="s">
+        <v>45</v>
+      </c>
+      <c r="B327" t="s">
+        <v>37</v>
+      </c>
+      <c r="C327" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D327" t="s">
+        <v>1</v>
+      </c>
+      <c r="E327" t="s">
+        <v>38</v>
+      </c>
+      <c r="F327">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="328" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A328" t="s">
+        <v>45</v>
+      </c>
+      <c r="B328" t="s">
+        <v>37</v>
+      </c>
+      <c r="C328" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D328" t="s">
+        <v>1</v>
+      </c>
+      <c r="E328" t="s">
+        <v>39</v>
+      </c>
+      <c r="F328">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="329" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A329" t="s">
+        <v>45</v>
+      </c>
+      <c r="B329" t="s">
+        <v>37</v>
+      </c>
+      <c r="C329" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D329" t="s">
+        <v>1</v>
+      </c>
+      <c r="E329" t="s">
+        <v>60</v>
+      </c>
+      <c r="F329">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="330" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A330" t="s">
+        <v>45</v>
+      </c>
+      <c r="B330" t="s">
+        <v>37</v>
+      </c>
+      <c r="C330" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D330" t="s">
+        <v>2</v>
+      </c>
+      <c r="E330" t="s">
+        <v>38</v>
+      </c>
+      <c r="F330">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="331" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A331" t="s">
+        <v>45</v>
+      </c>
+      <c r="B331" t="s">
+        <v>37</v>
+      </c>
+      <c r="C331" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D331" t="s">
+        <v>2</v>
+      </c>
+      <c r="E331" t="s">
+        <v>39</v>
+      </c>
+      <c r="F331">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="332" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A332" t="s">
+        <v>45</v>
+      </c>
+      <c r="B332" t="s">
+        <v>37</v>
+      </c>
+      <c r="C332" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D332" t="s">
+        <v>2</v>
+      </c>
+      <c r="E332" t="s">
+        <v>60</v>
+      </c>
+      <c r="F332">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="333" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A333" t="s">
+        <v>45</v>
+      </c>
+      <c r="B333" t="s">
+        <v>37</v>
+      </c>
+      <c r="C333" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D333" t="s">
+        <v>3</v>
+      </c>
+      <c r="E333" t="s">
+        <v>38</v>
+      </c>
+      <c r="F333">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="334" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A334" t="s">
+        <v>45</v>
+      </c>
+      <c r="B334" t="s">
+        <v>37</v>
+      </c>
+      <c r="C334" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D334" t="s">
+        <v>3</v>
+      </c>
+      <c r="E334" t="s">
+        <v>39</v>
+      </c>
+      <c r="F334">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="335" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A335" t="s">
+        <v>45</v>
+      </c>
+      <c r="B335" t="s">
+        <v>37</v>
+      </c>
+      <c r="C335" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D335" t="s">
+        <v>3</v>
+      </c>
+      <c r="E335" t="s">
+        <v>60</v>
+      </c>
+      <c r="F335">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="336" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A336" t="s">
+        <v>45</v>
+      </c>
+      <c r="B336" t="s">
+        <v>37</v>
+      </c>
+      <c r="C336" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D336" t="s">
+        <v>46</v>
+      </c>
+      <c r="E336" t="s">
+        <v>38</v>
+      </c>
+      <c r="F336">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="337" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A337" t="s">
+        <v>45</v>
+      </c>
+      <c r="B337" t="s">
+        <v>37</v>
+      </c>
+      <c r="C337" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D337" t="s">
+        <v>46</v>
+      </c>
+      <c r="E337" t="s">
+        <v>39</v>
+      </c>
+      <c r="F337">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="338" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A338" t="s">
+        <v>45</v>
+      </c>
+      <c r="B338" t="s">
+        <v>37</v>
+      </c>
+      <c r="C338" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D338" t="s">
+        <v>46</v>
+      </c>
+      <c r="E338" t="s">
+        <v>60</v>
+      </c>
+      <c r="F338">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="339" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A339" t="s">
+        <v>45</v>
+      </c>
+      <c r="B339" t="s">
+        <v>37</v>
+      </c>
+      <c r="C339" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D339" t="s">
+        <v>4</v>
+      </c>
+      <c r="E339" t="s">
+        <v>38</v>
+      </c>
+      <c r="F339">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="340" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A340" t="s">
+        <v>45</v>
+      </c>
+      <c r="B340" t="s">
+        <v>37</v>
+      </c>
+      <c r="C340" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D340" t="s">
+        <v>4</v>
+      </c>
+      <c r="E340" t="s">
+        <v>39</v>
+      </c>
+      <c r="F340">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="341" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A341" t="s">
+        <v>45</v>
+      </c>
+      <c r="B341" t="s">
+        <v>37</v>
+      </c>
+      <c r="C341" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D341" t="s">
+        <v>4</v>
+      </c>
+      <c r="E341" t="s">
+        <v>60</v>
+      </c>
+      <c r="F341">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="342" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A342" t="s">
+        <v>45</v>
+      </c>
+      <c r="B342" t="s">
+        <v>37</v>
+      </c>
+      <c r="C342" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D342" t="s">
+        <v>5</v>
+      </c>
+      <c r="E342" t="s">
+        <v>38</v>
+      </c>
+      <c r="F342">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="343" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A343" t="s">
+        <v>45</v>
+      </c>
+      <c r="B343" t="s">
+        <v>37</v>
+      </c>
+      <c r="C343" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D343" t="s">
+        <v>5</v>
+      </c>
+      <c r="E343" t="s">
+        <v>39</v>
+      </c>
+      <c r="F343">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="344" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A344" t="s">
+        <v>45</v>
+      </c>
+      <c r="B344" t="s">
+        <v>37</v>
+      </c>
+      <c r="C344" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D344" t="s">
+        <v>5</v>
+      </c>
+      <c r="E344" t="s">
+        <v>60</v>
+      </c>
+      <c r="F344">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="345" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A345" t="s">
+        <v>45</v>
+      </c>
+      <c r="B345" t="s">
+        <v>37</v>
+      </c>
+      <c r="C345" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D345" t="s">
+        <v>6</v>
+      </c>
+      <c r="E345" t="s">
+        <v>38</v>
+      </c>
+      <c r="F345">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="346" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A346" t="s">
+        <v>45</v>
+      </c>
+      <c r="B346" t="s">
+        <v>37</v>
+      </c>
+      <c r="C346" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D346" t="s">
+        <v>6</v>
+      </c>
+      <c r="E346" t="s">
+        <v>39</v>
+      </c>
+      <c r="F346">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="347" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A347" t="s">
+        <v>45</v>
+      </c>
+      <c r="B347" t="s">
+        <v>37</v>
+      </c>
+      <c r="C347" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D347" t="s">
+        <v>6</v>
+      </c>
+      <c r="E347" t="s">
+        <v>60</v>
+      </c>
+      <c r="F347">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="348" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A348" t="s">
+        <v>45</v>
+      </c>
+      <c r="B348" t="s">
+        <v>37</v>
+      </c>
+      <c r="C348" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D348" t="s">
+        <v>7</v>
+      </c>
+      <c r="E348" t="s">
+        <v>38</v>
+      </c>
+      <c r="F348">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="349" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A349" t="s">
+        <v>45</v>
+      </c>
+      <c r="B349" t="s">
+        <v>37</v>
+      </c>
+      <c r="C349" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D349" t="s">
+        <v>7</v>
+      </c>
+      <c r="E349" t="s">
+        <v>39</v>
+      </c>
+      <c r="F349">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="350" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A350" t="s">
+        <v>45</v>
+      </c>
+      <c r="B350" t="s">
+        <v>37</v>
+      </c>
+      <c r="C350" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D350" t="s">
+        <v>7</v>
+      </c>
+      <c r="E350" t="s">
+        <v>60</v>
+      </c>
+      <c r="F350">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="351" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A351" t="s">
+        <v>45</v>
+      </c>
+      <c r="B351" t="s">
+        <v>37</v>
+      </c>
+      <c r="C351" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D351" t="s">
+        <v>8</v>
+      </c>
+      <c r="E351" t="s">
+        <v>38</v>
+      </c>
+      <c r="F351">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="352" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A352" t="s">
+        <v>45</v>
+      </c>
+      <c r="B352" t="s">
+        <v>37</v>
+      </c>
+      <c r="C352" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D352" t="s">
+        <v>8</v>
+      </c>
+      <c r="E352" t="s">
+        <v>39</v>
+      </c>
+      <c r="F352">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="353" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A353" t="s">
+        <v>45</v>
+      </c>
+      <c r="B353" t="s">
+        <v>37</v>
+      </c>
+      <c r="C353" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D353" t="s">
+        <v>8</v>
+      </c>
+      <c r="E353" t="s">
+        <v>60</v>
+      </c>
+      <c r="F353">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="354" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A354" t="s">
+        <v>45</v>
+      </c>
+      <c r="B354" t="s">
+        <v>37</v>
+      </c>
+      <c r="C354" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D354" t="s">
+        <v>9</v>
+      </c>
+      <c r="E354" t="s">
+        <v>38</v>
+      </c>
+      <c r="F354">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="355" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A355" t="s">
+        <v>45</v>
+      </c>
+      <c r="B355" t="s">
+        <v>37</v>
+      </c>
+      <c r="C355" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D355" t="s">
+        <v>9</v>
+      </c>
+      <c r="E355" t="s">
+        <v>39</v>
+      </c>
+      <c r="F355">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="356" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A356" t="s">
+        <v>45</v>
+      </c>
+      <c r="B356" t="s">
+        <v>37</v>
+      </c>
+      <c r="C356" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D356" t="s">
+        <v>9</v>
+      </c>
+      <c r="E356" t="s">
+        <v>60</v>
+      </c>
+      <c r="F356">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="357" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A357" t="s">
+        <v>45</v>
+      </c>
+      <c r="B357" t="s">
+        <v>37</v>
+      </c>
+      <c r="C357" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D357" t="s">
+        <v>40</v>
+      </c>
+      <c r="E357" t="s">
+        <v>38</v>
+      </c>
+      <c r="F357">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="358" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A358" t="s">
+        <v>45</v>
+      </c>
+      <c r="B358" t="s">
+        <v>37</v>
+      </c>
+      <c r="C358" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D358" t="s">
+        <v>40</v>
+      </c>
+      <c r="E358" t="s">
+        <v>39</v>
+      </c>
+      <c r="F358">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="359" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A359" t="s">
+        <v>45</v>
+      </c>
+      <c r="B359" t="s">
+        <v>37</v>
+      </c>
+      <c r="C359" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D359" t="s">
+        <v>40</v>
+      </c>
+      <c r="E359" t="s">
+        <v>60</v>
+      </c>
+      <c r="F359">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="360" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A360" t="s">
+        <v>45</v>
+      </c>
+      <c r="B360" t="s">
+        <v>37</v>
+      </c>
+      <c r="C360" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D360" t="s">
+        <v>67</v>
+      </c>
+      <c r="E360" t="s">
+        <v>38</v>
+      </c>
+      <c r="F360">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="361" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A361" t="s">
+        <v>45</v>
+      </c>
+      <c r="B361" t="s">
+        <v>37</v>
+      </c>
+      <c r="C361" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D361" t="s">
+        <v>67</v>
+      </c>
+      <c r="E361" t="s">
+        <v>39</v>
+      </c>
+      <c r="F361">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="362" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A362" t="s">
+        <v>45</v>
+      </c>
+      <c r="B362" t="s">
+        <v>37</v>
+      </c>
+      <c r="C362" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D362" t="s">
+        <v>67</v>
+      </c>
+      <c r="E362" t="s">
+        <v>60</v>
+      </c>
+      <c r="F362">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="363" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A363" t="s">
+        <v>45</v>
+      </c>
+      <c r="B363" t="s">
+        <v>37</v>
+      </c>
+      <c r="C363" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D363" t="s">
+        <v>68</v>
+      </c>
+      <c r="E363" t="s">
+        <v>38</v>
+      </c>
+      <c r="F363">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="364" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A364" t="s">
+        <v>45</v>
+      </c>
+      <c r="B364" t="s">
+        <v>37</v>
+      </c>
+      <c r="C364" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D364" t="s">
+        <v>68</v>
+      </c>
+      <c r="E364" t="s">
+        <v>39</v>
+      </c>
+      <c r="F364">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="365" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A365" t="s">
+        <v>45</v>
+      </c>
+      <c r="B365" t="s">
+        <v>37</v>
+      </c>
+      <c r="C365" s="1">
+        <v>43914.75</v>
+      </c>
+      <c r="D365" t="s">
+        <v>68</v>
+      </c>
+      <c r="E365" t="s">
+        <v>60</v>
+      </c>
+      <c r="F365">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>